<commit_message>
add few fields and error report
</commit_message>
<xml_diff>
--- a/Web2.xlsx
+++ b/Web2.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>ProductCatalogID</t>
   </si>
@@ -108,15 +108,6 @@
     <t>Current stock</t>
   </si>
   <si>
-    <t>5116877-50227802194</t>
-  </si>
-  <si>
-    <t>5116877-37196116890</t>
-  </si>
-  <si>
-    <t>5116877-54522434970</t>
-  </si>
-  <si>
     <t>rubber bands</t>
   </si>
   <si>
@@ -126,31 +117,55 @@
     <t>Good Make</t>
   </si>
   <si>
-    <t>GS WORK -O-RING GASKET 140MM/160MM FOR CENTRAL LIGHT 1. GENERAL INFORMATION</t>
-  </si>
-  <si>
-    <t>http://mkp.gem.gov.in/rubber-bands/rubber-band-o-ring-gasket-140mm-160mm-central/p-5116877-50227802194-cat.html</t>
-  </si>
-  <si>
-    <t>https://admin-mkp.gem.gov.in/#!/catalog/new?bnid=home_offi_of45811733_fast_rubb&amp;gem_catalog_id=5116877-50227802194</t>
-  </si>
-  <si>
-    <t>Workstore 100202050014</t>
-  </si>
-  <si>
-    <t>http://mkp.gem.gov.in/rubber-bands/nylon-rubber-band-4-inch-assorted-colours-500/p-5116877-37196116890-cat.html</t>
-  </si>
-  <si>
-    <t>https://admin-mkp.gem.gov.in/#!/catalog/new?bnid=home_offi_of45811733_fast_rubb&amp;gem_catalog_id=5116877-37196116890</t>
-  </si>
-  <si>
-    <t>Workstore 100202050015</t>
-  </si>
-  <si>
-    <t>http://mkp.gem.gov.in/rubber-bands/nylon-rubber-band-2-inch-assorted-colours-500/p-5116877-54522434970-cat.html</t>
-  </si>
-  <si>
-    <t>https://admin-mkp.gem.gov.in/#!/catalog/new?bnid=home_offi_of45811733_fast_rubb&amp;gem_catalog_id=5116877-54522434970</t>
+    <t>5116877-32863368197</t>
+  </si>
+  <si>
+    <t>NYLON RUBBER BAND Pkt 500gm</t>
+  </si>
+  <si>
+    <t>Ekam</t>
+  </si>
+  <si>
+    <t>http://mkp.gem.gov.in/rubber-bands/nylon-rubber-band-pkt-500gm/p-5116877-32863368197-cat.html</t>
+  </si>
+  <si>
+    <t>https://admin-mkp.gem.gov.in/#!/catalog/new?bnid=home_offi_of45811733_fast_rubb&amp;gem_catalog_id=5116877-32863368197</t>
+  </si>
+  <si>
+    <t>5116877-15821908934</t>
+  </si>
+  <si>
+    <t>GOOD MAKE RUBBER BAND</t>
+  </si>
+  <si>
+    <t>http://mkp.gem.gov.in/rubber-bands/rubber-band-big-size/p-5116877-15821908934-cat.html</t>
+  </si>
+  <si>
+    <t>https://admin-mkp.gem.gov.in/#!/catalog/new?bnid=home_offi_of45811733_fast_rubb&amp;gem_catalog_id=5116877-15821908934</t>
+  </si>
+  <si>
+    <t>5116877-17154744803</t>
+  </si>
+  <si>
+    <t>R-73947</t>
+  </si>
+  <si>
+    <t>http://mkp.gem.gov.in/office-equipment-accessories-supplies/rubber-bands/p-5116877-17154744803-cat.html</t>
+  </si>
+  <si>
+    <t>https://admin-mkp.gem.gov.in/#!/catalog/new?bnid=home_offi_of45811733_fast_rubb&amp;gem_catalog_id=5116877-17154744803</t>
+  </si>
+  <si>
+    <t>5116877-92981260387</t>
+  </si>
+  <si>
+    <t>RUBBER BAND GOOD MAKE</t>
+  </si>
+  <si>
+    <t>http://mkp.gem.gov.in/rubber-bands/rubber-band-good-make/p-5116877-92981260387-cat.html</t>
+  </si>
+  <si>
+    <t>https://admin-mkp.gem.gov.in/#!/catalog/new?bnid=home_offi_of45811733_fast_rubb&amp;gem_catalog_id=5116877-92981260387</t>
   </si>
 </sst>
 </file>
@@ -537,7 +552,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,7 +563,7 @@
   <dimension ref="A1:X126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:V4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,25 +654,25 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>32</v>
       </c>
       <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
-        <v>35</v>
-      </c>
       <c r="G2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -678,19 +693,19 @@
         <v>4016</v>
       </c>
       <c r="O2">
-        <v>600</v>
+        <v>312</v>
       </c>
       <c r="P2">
-        <v>315.31</v>
+        <v>279.99</v>
       </c>
       <c r="S2" t="s">
         <v>23</v>
       </c>
       <c r="T2">
-        <v>51421</v>
+        <v>51415</v>
       </c>
       <c r="U2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="V2">
         <v>3</v>
@@ -698,16 +713,16 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E3" t="s">
         <v>37</v>
@@ -716,7 +731,7 @@
         <v>38</v>
       </c>
       <c r="G3" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H3" t="s">
         <v>12</v>
@@ -737,19 +752,19 @@
         <v>4016</v>
       </c>
       <c r="O3">
-        <v>319</v>
+        <v>480</v>
       </c>
       <c r="P3">
-        <v>284</v>
+        <v>398.99</v>
       </c>
       <c r="S3" t="s">
         <v>23</v>
       </c>
       <c r="T3">
-        <v>51423</v>
+        <v>51417</v>
       </c>
       <c r="U3">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V3">
         <v>3</v>
@@ -757,25 +772,25 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
         <v>29</v>
       </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -796,28 +811,82 @@
         <v>4016</v>
       </c>
       <c r="O4">
-        <v>500</v>
+        <v>430</v>
       </c>
       <c r="P4">
-        <v>279.97000000000003</v>
+        <v>380.99</v>
       </c>
       <c r="S4" t="s">
         <v>23</v>
       </c>
       <c r="T4">
-        <v>51419</v>
+        <v>51418</v>
       </c>
       <c r="U4">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="V4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1">
+        <v>44166</v>
+      </c>
+      <c r="J5" s="1">
+        <v>44166</v>
+      </c>
+      <c r="K5" s="1">
+        <v>46022</v>
+      </c>
+      <c r="L5" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5">
+        <v>4016</v>
+      </c>
+      <c r="O5">
+        <v>430</v>
+      </c>
+      <c r="P5">
+        <v>380.99</v>
+      </c>
+      <c r="S5" t="s">
+        <v>23</v>
+      </c>
+      <c r="T5">
+        <v>51420</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="V5">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="I6" s="1"/>

</xml_diff>